<commit_message>
Added a tutorial on pQTLs.
</commit_message>
<xml_diff>
--- a/votes/votes.xlsx
+++ b/votes/votes.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\IBIP21\votes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{9F28EC82-B238-48FE-A84F-BCBDE9ABF78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C59876A-05A2-4A8D-BDF6-09E43326772B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Please try to rate how much the knowledge you acquired since yesterday could help you to review proteomics datasets you plan to analyze in the near future</t>
   </si>
@@ -53,12 +53,21 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>How comfortable are you using Jupyter QC notebooks to review the quality of MS/MS identifications</t>
+  </si>
+  <si>
+    <t>How comfortable are you about using the 'git pull' command to update the IBIP21 folder</t>
+  </si>
+  <si>
+    <t>If a student asks you how to find the consequence of a variant on a protein, how confident do you feel about explaining them how to find it in Ensembl?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -403,11 +412,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,6 +535,80 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>